<commit_message>
Enabled the ability to add new seasons to the dataset.
</commit_message>
<xml_diff>
--- a/data/volley_stats.xlsx
+++ b/data/volley_stats.xlsx
@@ -454,10 +454,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -467,17 +467,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1" s="4">
-      <c r="A1" s="6" t="inlineStr">
-        <is>
-          <t>Season No.</t>
-        </is>
-      </c>
-      <c r="B1" s="6" t="inlineStr">
-        <is>
-          <t>Player Count</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Number of Seasons</t>
         </is>
@@ -485,148 +475,241 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" ht="30" customHeight="1" s="4">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>Season No.</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>Player Count</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B4" t="n">
         <v>10</v>
       </c>
-      <c r="K2" t="n">
+    </row>
+    <row r="5" ht="15.75" customHeight="1" s="4" thickBot="1">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Player Names</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="30.75" customHeight="1" s="4" thickBot="1">
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t>Brandon Chan</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>Callum Ashton</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>Daniel Park</t>
+        </is>
+      </c>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>Deidre Truong</t>
+        </is>
+      </c>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t>Edward Kang</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>Kevin Ma</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
+          <t>Kevin Tang</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>Lachlan Denham</t>
+        </is>
+      </c>
+      <c r="I6" s="5" t="inlineStr">
+        <is>
+          <t>Mimi Chen</t>
+        </is>
+      </c>
+      <c r="J6" s="5" t="inlineStr">
+        <is>
+          <t>Will Ouyang</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="30" customHeight="1" s="4">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>Season No.</t>
+        </is>
+      </c>
+      <c r="B8" s="6" t="inlineStr">
+        <is>
+          <t>Player Count</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1" s="4" thickBot="1">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Player Names</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="30.75" customHeight="1" s="4" thickBot="1">
+      <c r="A11" s="5" t="inlineStr">
+        <is>
+          <t>Brandon Chan</t>
+        </is>
+      </c>
+      <c r="B11" s="5" t="inlineStr">
+        <is>
+          <t>Callum Ashton</t>
+        </is>
+      </c>
+      <c r="C11" s="5" t="inlineStr">
+        <is>
+          <t>Daniel Park</t>
+        </is>
+      </c>
+      <c r="D11" s="5" t="inlineStr">
+        <is>
+          <t>Deidre Truong</t>
+        </is>
+      </c>
+      <c r="E11" s="5" t="inlineStr">
+        <is>
+          <t>Edward Kang</t>
+        </is>
+      </c>
+      <c r="F11" s="5" t="inlineStr">
+        <is>
+          <t>Kevin Ma</t>
+        </is>
+      </c>
+      <c r="G11" s="5" t="inlineStr">
+        <is>
+          <t>Kevin Tang</t>
+        </is>
+      </c>
+      <c r="H11" s="5" t="inlineStr">
+        <is>
+          <t>Lachlan Denham</t>
+        </is>
+      </c>
+      <c r="I11" s="5" t="inlineStr">
+        <is>
+          <t>Mimi Chen</t>
+        </is>
+      </c>
+      <c r="J11" s="5" t="inlineStr">
+        <is>
+          <t>Will Ouyang</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="30" customHeight="1" s="4">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>Season No.</t>
+        </is>
+      </c>
+      <c r="B13" s="6" t="inlineStr">
+        <is>
+          <t>Player Count</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1" s="4" thickBot="1">
-      <c r="A3" t="inlineStr">
+      <c r="B14" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1" s="4" thickBot="1">
+      <c r="A15" t="inlineStr">
         <is>
           <t>Player Names</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="30.75" customHeight="1" s="4" thickBot="1">
-      <c r="A4" s="5" t="inlineStr">
+    <row r="16" ht="30.75" customHeight="1" s="4" thickBot="1">
+      <c r="A16" s="5" t="inlineStr">
         <is>
           <t>Brandon Chan</t>
         </is>
       </c>
-      <c r="B4" s="5" t="inlineStr">
+      <c r="B16" s="5" t="inlineStr">
         <is>
           <t>Callum Ashton</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr">
+      <c r="C16" s="5" t="inlineStr">
         <is>
           <t>Daniel Park</t>
         </is>
       </c>
-      <c r="D4" s="5" t="inlineStr">
+      <c r="D16" s="5" t="inlineStr">
         <is>
           <t>Deidre Truong</t>
         </is>
       </c>
-      <c r="E4" s="5" t="inlineStr">
+      <c r="E16" s="5" t="inlineStr">
         <is>
           <t>Edward Kang</t>
         </is>
       </c>
-      <c r="F4" s="5" t="inlineStr">
+      <c r="F16" s="5" t="inlineStr">
         <is>
           <t>Kevin Ma</t>
         </is>
       </c>
-      <c r="G4" s="5" t="inlineStr">
+      <c r="G16" s="5" t="inlineStr">
         <is>
           <t>Kevin Tang</t>
         </is>
       </c>
-      <c r="H4" s="5" t="inlineStr">
+      <c r="H16" s="5" t="inlineStr">
         <is>
           <t>Lachlan Denham</t>
         </is>
       </c>
-      <c r="I4" s="5" t="inlineStr">
+      <c r="I16" s="5" t="inlineStr">
         <is>
           <t>Mimi Chen</t>
         </is>
       </c>
-      <c r="J4" s="5" t="inlineStr">
-        <is>
-          <t>Will Ouyang</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" ht="30" customHeight="1" s="4">
-      <c r="A6" s="6" t="inlineStr">
-        <is>
-          <t>Season No.</t>
-        </is>
-      </c>
-      <c r="B6" s="6" t="inlineStr">
-        <is>
-          <t>Player Count</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1" s="4" thickBot="1">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Player Names</t>
-        </is>
-      </c>
-    </row>
-    <row r="9" ht="30.75" customHeight="1" s="4" thickBot="1">
-      <c r="A9" s="5" t="inlineStr">
-        <is>
-          <t>Brandon Chan</t>
-        </is>
-      </c>
-      <c r="B9" s="5" t="inlineStr">
-        <is>
-          <t>Callum Ashton</t>
-        </is>
-      </c>
-      <c r="C9" s="5" t="inlineStr">
-        <is>
-          <t>Daniel Park</t>
-        </is>
-      </c>
-      <c r="D9" s="5" t="inlineStr">
-        <is>
-          <t>Deidre Truong</t>
-        </is>
-      </c>
-      <c r="E9" s="5" t="inlineStr">
-        <is>
-          <t>Edward Kang</t>
-        </is>
-      </c>
-      <c r="F9" s="5" t="inlineStr">
-        <is>
-          <t>Kevin Ma</t>
-        </is>
-      </c>
-      <c r="G9" s="5" t="inlineStr">
-        <is>
-          <t>Kevin Tang</t>
-        </is>
-      </c>
-      <c r="H9" s="5" t="inlineStr">
-        <is>
-          <t>Lachlan Denham</t>
-        </is>
-      </c>
-      <c r="I9" s="5" t="inlineStr">
-        <is>
-          <t>Mimi Chen</t>
-        </is>
-      </c>
-      <c r="J9" s="5" t="inlineStr">
+      <c r="J16" s="5" t="inlineStr">
         <is>
           <t>Will Ouyang</t>
         </is>
@@ -646,7 +729,7 @@
   </sheetPr>
   <dimension ref="A1:T142"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A12"/>
     </sheetView>
   </sheetViews>
@@ -10244,7 +10327,7 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
The add season function now moves a basic template over to the newly created worksheet.
</commit_message>
<xml_diff>
--- a/data/volley_stats.xlsx
+++ b/data/volley_stats.xlsx
@@ -9,7 +9,6 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Team Info" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Season 1" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Season 2" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Season 3" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -80,10 +79,10 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -454,31 +453,146 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:AD16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10.7109375" customWidth="1" style="4" min="1" max="1"/>
-    <col width="12.140625" customWidth="1" style="4" min="2" max="2"/>
+    <col width="10.7109375" customWidth="1" style="5" min="1" max="1"/>
+    <col width="12.140625" customWidth="1" style="5" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" customHeight="1" s="4">
+    <row r="1" ht="30" customHeight="1" s="5" thickBot="1">
       <c r="A1" t="inlineStr">
         <is>
           <t>Number of Seasons</t>
         </is>
       </c>
-    </row>
-    <row r="2">
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Team Name</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>WEEK</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" ht="30" customHeight="1" s="4">
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>We Take Those</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>VS 'TEAM'</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
+        <is>
+          <t>Serve Error</t>
+        </is>
+      </c>
+      <c r="M2" s="1" t="inlineStr">
+        <is>
+          <t>Serve Success</t>
+        </is>
+      </c>
+      <c r="N2" s="1" t="inlineStr">
+        <is>
+          <t>Serve %</t>
+        </is>
+      </c>
+      <c r="O2" s="1" t="inlineStr">
+        <is>
+          <t>Receive Errors</t>
+        </is>
+      </c>
+      <c r="P2" s="1" t="inlineStr">
+        <is>
+          <t>Receive Passes</t>
+        </is>
+      </c>
+      <c r="Q2" s="1" t="inlineStr">
+        <is>
+          <t>Receive %</t>
+        </is>
+      </c>
+      <c r="R2" s="1" t="inlineStr">
+        <is>
+          <t>Set Errors</t>
+        </is>
+      </c>
+      <c r="S2" s="1" t="inlineStr">
+        <is>
+          <t>Set Success</t>
+        </is>
+      </c>
+      <c r="T2" s="1" t="inlineStr">
+        <is>
+          <t>Set %</t>
+        </is>
+      </c>
+      <c r="U2" s="1" t="inlineStr">
+        <is>
+          <t>Spike Errors</t>
+        </is>
+      </c>
+      <c r="V2" s="1" t="inlineStr">
+        <is>
+          <t>Spike Success</t>
+        </is>
+      </c>
+      <c r="W2" s="1" t="inlineStr">
+        <is>
+          <t>Hit %</t>
+        </is>
+      </c>
+      <c r="X2" s="1" t="inlineStr">
+        <is>
+          <t>Tip Errors</t>
+        </is>
+      </c>
+      <c r="Y2" s="1" t="inlineStr">
+        <is>
+          <t>Tip Success</t>
+        </is>
+      </c>
+      <c r="Z2" s="1" t="inlineStr">
+        <is>
+          <t>Tip %</t>
+        </is>
+      </c>
+      <c r="AA2" s="1" t="inlineStr">
+        <is>
+          <t>Block Errors</t>
+        </is>
+      </c>
+      <c r="AB2" s="1" t="inlineStr">
+        <is>
+          <t>Block Success</t>
+        </is>
+      </c>
+      <c r="AC2" s="1" t="inlineStr">
+        <is>
+          <t>Block %</t>
+        </is>
+      </c>
+      <c r="AD2" s="1" t="inlineStr">
+        <is>
+          <t>Faults</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="30" customHeight="1" s="5">
       <c r="A3" s="6" t="inlineStr">
         <is>
           <t>Season No.</t>
@@ -498,66 +612,66 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="5" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A5" t="inlineStr">
         <is>
           <t>Player Names</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="30.75" customHeight="1" s="4" thickBot="1">
-      <c r="A6" s="5" t="inlineStr">
+    <row r="6" ht="30.75" customHeight="1" s="5" thickBot="1">
+      <c r="A6" s="4" t="inlineStr">
         <is>
           <t>Brandon Chan</t>
         </is>
       </c>
-      <c r="B6" s="5" t="inlineStr">
+      <c r="B6" s="4" t="inlineStr">
         <is>
           <t>Callum Ashton</t>
         </is>
       </c>
-      <c r="C6" s="5" t="inlineStr">
+      <c r="C6" s="4" t="inlineStr">
         <is>
           <t>Daniel Park</t>
         </is>
       </c>
-      <c r="D6" s="5" t="inlineStr">
+      <c r="D6" s="4" t="inlineStr">
         <is>
           <t>Deidre Truong</t>
         </is>
       </c>
-      <c r="E6" s="5" t="inlineStr">
+      <c r="E6" s="4" t="inlineStr">
         <is>
           <t>Edward Kang</t>
         </is>
       </c>
-      <c r="F6" s="5" t="inlineStr">
+      <c r="F6" s="4" t="inlineStr">
         <is>
           <t>Kevin Ma</t>
         </is>
       </c>
-      <c r="G6" s="5" t="inlineStr">
+      <c r="G6" s="4" t="inlineStr">
         <is>
           <t>Kevin Tang</t>
         </is>
       </c>
-      <c r="H6" s="5" t="inlineStr">
+      <c r="H6" s="4" t="inlineStr">
         <is>
           <t>Lachlan Denham</t>
         </is>
       </c>
-      <c r="I6" s="5" t="inlineStr">
+      <c r="I6" s="4" t="inlineStr">
         <is>
           <t>Mimi Chen</t>
         </is>
       </c>
-      <c r="J6" s="5" t="inlineStr">
+      <c r="J6" s="4" t="inlineStr">
         <is>
           <t>Will Ouyang</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="30" customHeight="1" s="4">
+    <row r="8" ht="30" customHeight="1" s="5">
       <c r="A8" s="6" t="inlineStr">
         <is>
           <t>Season No.</t>
@@ -574,146 +688,44 @@
         <v>2</v>
       </c>
       <c r="B9" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1" s="4" thickBot="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1" s="5">
       <c r="A10" t="inlineStr">
         <is>
           <t>Player Names</t>
         </is>
       </c>
     </row>
-    <row r="11" ht="30.75" customHeight="1" s="4" thickBot="1">
-      <c r="A11" s="5" t="inlineStr">
-        <is>
-          <t>Brandon Chan</t>
-        </is>
-      </c>
-      <c r="B11" s="5" t="inlineStr">
-        <is>
-          <t>Callum Ashton</t>
-        </is>
-      </c>
-      <c r="C11" s="5" t="inlineStr">
-        <is>
-          <t>Daniel Park</t>
-        </is>
-      </c>
-      <c r="D11" s="5" t="inlineStr">
-        <is>
-          <t>Deidre Truong</t>
-        </is>
-      </c>
-      <c r="E11" s="5" t="inlineStr">
-        <is>
-          <t>Edward Kang</t>
-        </is>
-      </c>
-      <c r="F11" s="5" t="inlineStr">
-        <is>
-          <t>Kevin Ma</t>
-        </is>
-      </c>
-      <c r="G11" s="5" t="inlineStr">
-        <is>
-          <t>Kevin Tang</t>
-        </is>
-      </c>
-      <c r="H11" s="5" t="inlineStr">
-        <is>
-          <t>Lachlan Denham</t>
-        </is>
-      </c>
-      <c r="I11" s="5" t="inlineStr">
-        <is>
-          <t>Mimi Chen</t>
-        </is>
-      </c>
-      <c r="J11" s="5" t="inlineStr">
-        <is>
-          <t>Will Ouyang</t>
-        </is>
-      </c>
-    </row>
-    <row r="13" ht="30" customHeight="1" s="4">
-      <c r="A13" s="6" t="inlineStr">
-        <is>
-          <t>Season No.</t>
-        </is>
-      </c>
-      <c r="B13" s="6" t="inlineStr">
-        <is>
-          <t>Player Count</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>3</v>
-      </c>
-      <c r="B14" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1" s="4" thickBot="1">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Player Names</t>
-        </is>
-      </c>
-    </row>
-    <row r="16" ht="30.75" customHeight="1" s="4" thickBot="1">
-      <c r="A16" s="5" t="inlineStr">
-        <is>
-          <t>Brandon Chan</t>
-        </is>
-      </c>
-      <c r="B16" s="5" t="inlineStr">
-        <is>
-          <t>Callum Ashton</t>
-        </is>
-      </c>
-      <c r="C16" s="5" t="inlineStr">
-        <is>
-          <t>Daniel Park</t>
-        </is>
-      </c>
-      <c r="D16" s="5" t="inlineStr">
-        <is>
-          <t>Deidre Truong</t>
-        </is>
-      </c>
-      <c r="E16" s="5" t="inlineStr">
-        <is>
-          <t>Edward Kang</t>
-        </is>
-      </c>
-      <c r="F16" s="5" t="inlineStr">
-        <is>
-          <t>Kevin Ma</t>
-        </is>
-      </c>
-      <c r="G16" s="5" t="inlineStr">
-        <is>
-          <t>Kevin Tang</t>
-        </is>
-      </c>
-      <c r="H16" s="5" t="inlineStr">
-        <is>
-          <t>Lachlan Denham</t>
-        </is>
-      </c>
-      <c r="I16" s="5" t="inlineStr">
-        <is>
-          <t>Mimi Chen</t>
-        </is>
-      </c>
-      <c r="J16" s="5" t="inlineStr">
-        <is>
-          <t>Will Ouyang</t>
-        </is>
-      </c>
+    <row r="11" ht="30.75" customHeight="1" s="5">
+      <c r="A11" s="6" t="n"/>
+      <c r="B11" s="6" t="n"/>
+      <c r="C11" s="6" t="n"/>
+      <c r="D11" s="6" t="n"/>
+      <c r="E11" s="6" t="n"/>
+      <c r="F11" s="6" t="n"/>
+      <c r="G11" s="6" t="n"/>
+      <c r="H11" s="6" t="n"/>
+      <c r="I11" s="6" t="n"/>
+      <c r="J11" s="6" t="n"/>
+    </row>
+    <row r="13" ht="30" customHeight="1" s="5">
+      <c r="A13" s="6" t="n"/>
+      <c r="B13" s="6" t="n"/>
+    </row>
+    <row r="15" ht="15.75" customHeight="1" s="5"/>
+    <row r="16" ht="30.75" customHeight="1" s="5">
+      <c r="A16" s="6" t="n"/>
+      <c r="B16" s="6" t="n"/>
+      <c r="C16" s="6" t="n"/>
+      <c r="D16" s="6" t="n"/>
+      <c r="E16" s="6" t="n"/>
+      <c r="F16" s="6" t="n"/>
+      <c r="G16" s="6" t="n"/>
+      <c r="H16" s="6" t="n"/>
+      <c r="I16" s="6" t="n"/>
+      <c r="J16" s="6" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -729,20 +741,20 @@
   </sheetPr>
   <dimension ref="A1:T142"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="1" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A1" t="inlineStr">
         <is>
           <t>WEEK#</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="39.75" customHeight="1" s="4" thickBot="1">
+    <row r="2" ht="39.75" customHeight="1" s="5" thickBot="1">
       <c r="A2" s="1" t="inlineStr">
         <is>
           <t>VS 'TEAM'</t>
@@ -844,7 +856,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="3" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A3" s="1" t="inlineStr">
         <is>
           <t>Brandon Chan</t>
@@ -920,7 +932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="4" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A4" s="1" t="inlineStr">
         <is>
           <t>Callum Ashton</t>
@@ -996,7 +1008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="5" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>Daniel Park</t>
@@ -1072,7 +1084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="6" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A6" s="1" t="inlineStr">
         <is>
           <t>Deidre Truong</t>
@@ -1148,7 +1160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="7" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A7" s="1" t="inlineStr">
         <is>
           <t>Edward Kang</t>
@@ -1224,7 +1236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="8" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A8" s="1" t="inlineStr">
         <is>
           <t>Kevin Ma</t>
@@ -1300,7 +1312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="9" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A9" s="1" t="inlineStr">
         <is>
           <t>Kevin Tang</t>
@@ -1376,7 +1388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="10" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A10" s="1" t="inlineStr">
         <is>
           <t>Lachlan Denham</t>
@@ -1452,7 +1464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="11" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A11" s="1" t="inlineStr">
         <is>
           <t>Mimi Chen</t>
@@ -1528,7 +1540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="12" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A12" s="1" t="inlineStr">
         <is>
           <t>Will Ouyang</t>
@@ -1604,14 +1616,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="14" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A14" t="inlineStr">
         <is>
           <t>WEEK#</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="39.75" customHeight="1" s="4" thickBot="1">
+    <row r="15" ht="39.75" customHeight="1" s="5" thickBot="1">
       <c r="A15" s="1" t="inlineStr">
         <is>
           <t>VS 'TEAM'</t>
@@ -1713,7 +1725,7 @@
         </is>
       </c>
     </row>
-    <row r="16" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="16" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A16" s="1" t="inlineStr">
         <is>
           <t>Brandon Chan</t>
@@ -1789,7 +1801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="17" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A17" s="1" t="inlineStr">
         <is>
           <t>Callum Ashton</t>
@@ -1865,7 +1877,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="18" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A18" s="1" t="inlineStr">
         <is>
           <t>Daniel Park</t>
@@ -1941,7 +1953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="19" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A19" s="1" t="inlineStr">
         <is>
           <t>Deidre Truong</t>
@@ -2017,7 +2029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="20" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A20" s="1" t="inlineStr">
         <is>
           <t>Edward Kang</t>
@@ -2093,7 +2105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="21" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A21" s="1" t="inlineStr">
         <is>
           <t>Kevin Ma</t>
@@ -2169,7 +2181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="22" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A22" s="1" t="inlineStr">
         <is>
           <t>Kevin Tang</t>
@@ -2245,7 +2257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="23" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A23" s="1" t="inlineStr">
         <is>
           <t>Lachlan Denham</t>
@@ -2321,7 +2333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="24" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A24" s="1" t="inlineStr">
         <is>
           <t>Mimi Chen</t>
@@ -2397,7 +2409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="25" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A25" s="1" t="inlineStr">
         <is>
           <t>Will Ouyang</t>
@@ -2473,14 +2485,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="27" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A27" t="inlineStr">
         <is>
           <t>WEEK#</t>
         </is>
       </c>
     </row>
-    <row r="28" ht="39.75" customHeight="1" s="4" thickBot="1">
+    <row r="28" ht="39.75" customHeight="1" s="5" thickBot="1">
       <c r="A28" s="1" t="inlineStr">
         <is>
           <t>VS 'TEAM'</t>
@@ -2582,7 +2594,7 @@
         </is>
       </c>
     </row>
-    <row r="29" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="29" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A29" s="1" t="inlineStr">
         <is>
           <t>Brandon Chan</t>
@@ -2658,7 +2670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="30" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A30" s="1" t="inlineStr">
         <is>
           <t>Callum Ashton</t>
@@ -2734,7 +2746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="31" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A31" s="1" t="inlineStr">
         <is>
           <t>Daniel Park</t>
@@ -2810,7 +2822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="32" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A32" s="1" t="inlineStr">
         <is>
           <t>Deidre Truong</t>
@@ -2886,7 +2898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="33" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A33" s="1" t="inlineStr">
         <is>
           <t>Edward Kang</t>
@@ -2962,7 +2974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="34" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A34" s="1" t="inlineStr">
         <is>
           <t>Kevin Ma</t>
@@ -3038,7 +3050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="35" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A35" s="1" t="inlineStr">
         <is>
           <t>Kevin Tang</t>
@@ -3114,7 +3126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="36" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A36" s="1" t="inlineStr">
         <is>
           <t>Lachlan Denham</t>
@@ -3190,7 +3202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="37" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A37" s="1" t="inlineStr">
         <is>
           <t>Mimi Chen</t>
@@ -3266,7 +3278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="38" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A38" s="1" t="inlineStr">
         <is>
           <t>Will Ouyang</t>
@@ -3342,14 +3354,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="40" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A40" t="inlineStr">
         <is>
           <t>WEEK#</t>
         </is>
       </c>
     </row>
-    <row r="41" ht="39.75" customHeight="1" s="4" thickBot="1">
+    <row r="41" ht="39.75" customHeight="1" s="5" thickBot="1">
       <c r="A41" s="1" t="inlineStr">
         <is>
           <t>VS 'TEAM'</t>
@@ -3451,7 +3463,7 @@
         </is>
       </c>
     </row>
-    <row r="42" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="42" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A42" s="1" t="inlineStr">
         <is>
           <t>Brandon Chan</t>
@@ -3527,7 +3539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="43" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A43" s="1" t="inlineStr">
         <is>
           <t>Callum Ashton</t>
@@ -3603,7 +3615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="44" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A44" s="1" t="inlineStr">
         <is>
           <t>Daniel Park</t>
@@ -3679,7 +3691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="45" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A45" s="1" t="inlineStr">
         <is>
           <t>Deidre Truong</t>
@@ -3755,7 +3767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="46" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A46" s="1" t="inlineStr">
         <is>
           <t>Edward Kang</t>
@@ -3831,7 +3843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="47" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A47" s="1" t="inlineStr">
         <is>
           <t>Kevin Ma</t>
@@ -3907,7 +3919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="48" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A48" s="1" t="inlineStr">
         <is>
           <t>Kevin Tang</t>
@@ -3983,7 +3995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="49" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A49" s="1" t="inlineStr">
         <is>
           <t>Lachlan Denham</t>
@@ -4059,7 +4071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="50" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A50" s="1" t="inlineStr">
         <is>
           <t>Mimi Chen</t>
@@ -4135,7 +4147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="51" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A51" s="1" t="inlineStr">
         <is>
           <t>Will Ouyang</t>
@@ -4211,14 +4223,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="53" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A53" t="inlineStr">
         <is>
           <t>WEEK#</t>
         </is>
       </c>
     </row>
-    <row r="54" ht="39.75" customHeight="1" s="4" thickBot="1">
+    <row r="54" ht="39.75" customHeight="1" s="5" thickBot="1">
       <c r="A54" s="1" t="inlineStr">
         <is>
           <t>VS 'TEAM'</t>
@@ -4320,7 +4332,7 @@
         </is>
       </c>
     </row>
-    <row r="55" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="55" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A55" s="1" t="inlineStr">
         <is>
           <t>Brandon Chan</t>
@@ -4396,7 +4408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="56" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A56" s="1" t="inlineStr">
         <is>
           <t>Callum Ashton</t>
@@ -4472,7 +4484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="57" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A57" s="1" t="inlineStr">
         <is>
           <t>Daniel Park</t>
@@ -4548,7 +4560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="58" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A58" s="1" t="inlineStr">
         <is>
           <t>Deidre Truong</t>
@@ -4624,7 +4636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="59" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A59" s="1" t="inlineStr">
         <is>
           <t>Edward Kang</t>
@@ -4700,7 +4712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="60" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A60" s="1" t="inlineStr">
         <is>
           <t>Kevin Ma</t>
@@ -4776,7 +4788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="61" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A61" s="1" t="inlineStr">
         <is>
           <t>Kevin Tang</t>
@@ -4852,7 +4864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="62" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A62" s="1" t="inlineStr">
         <is>
           <t>Lachlan Denham</t>
@@ -4928,7 +4940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="63" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A63" s="1" t="inlineStr">
         <is>
           <t>Mimi Chen</t>
@@ -5004,7 +5016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="64" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A64" s="1" t="inlineStr">
         <is>
           <t>Will Ouyang</t>
@@ -5080,14 +5092,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="66" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A66" t="inlineStr">
         <is>
           <t>WEEK#</t>
         </is>
       </c>
     </row>
-    <row r="67" ht="39.75" customHeight="1" s="4" thickBot="1">
+    <row r="67" ht="39.75" customHeight="1" s="5" thickBot="1">
       <c r="A67" s="1" t="inlineStr">
         <is>
           <t>VS 'TEAM'</t>
@@ -5189,7 +5201,7 @@
         </is>
       </c>
     </row>
-    <row r="68" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="68" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A68" s="1" t="inlineStr">
         <is>
           <t>Brandon Chan</t>
@@ -5265,7 +5277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="69" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A69" s="1" t="inlineStr">
         <is>
           <t>Callum Ashton</t>
@@ -5341,7 +5353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="70" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A70" s="1" t="inlineStr">
         <is>
           <t>Daniel Park</t>
@@ -5417,7 +5429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="71" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A71" s="1" t="inlineStr">
         <is>
           <t>Deidre Truong</t>
@@ -5493,7 +5505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="72" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A72" s="1" t="inlineStr">
         <is>
           <t>Edward Kang</t>
@@ -5569,7 +5581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="73" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A73" s="1" t="inlineStr">
         <is>
           <t>Kevin Ma</t>
@@ -5645,7 +5657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="74" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A74" s="1" t="inlineStr">
         <is>
           <t>Kevin Tang</t>
@@ -5721,7 +5733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="75" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A75" s="1" t="inlineStr">
         <is>
           <t>Lachlan Denham</t>
@@ -5797,7 +5809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="76" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A76" s="1" t="inlineStr">
         <is>
           <t>Mimi Chen</t>
@@ -5873,7 +5885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="77" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A77" s="1" t="inlineStr">
         <is>
           <t>Will Ouyang</t>
@@ -5949,14 +5961,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="79" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A79" t="inlineStr">
         <is>
           <t>WEEK#</t>
         </is>
       </c>
     </row>
-    <row r="80" ht="39.75" customHeight="1" s="4" thickBot="1">
+    <row r="80" ht="39.75" customHeight="1" s="5" thickBot="1">
       <c r="A80" s="1" t="inlineStr">
         <is>
           <t>VS 'TEAM'</t>
@@ -6058,7 +6070,7 @@
         </is>
       </c>
     </row>
-    <row r="81" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="81" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A81" s="1" t="inlineStr">
         <is>
           <t>Brandon Chan</t>
@@ -6134,7 +6146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="82" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A82" s="1" t="inlineStr">
         <is>
           <t>Callum Ashton</t>
@@ -6210,7 +6222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="83" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A83" s="1" t="inlineStr">
         <is>
           <t>Daniel Park</t>
@@ -6286,7 +6298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="84" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A84" s="1" t="inlineStr">
         <is>
           <t>Deidre Truong</t>
@@ -6362,7 +6374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="85" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A85" s="1" t="inlineStr">
         <is>
           <t>Edward Kang</t>
@@ -6438,7 +6450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="86" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A86" s="1" t="inlineStr">
         <is>
           <t>Kevin Ma</t>
@@ -6514,7 +6526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="87" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A87" s="1" t="inlineStr">
         <is>
           <t>Kevin Tang</t>
@@ -6590,7 +6602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="88" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A88" s="1" t="inlineStr">
         <is>
           <t>Lachlan Denham</t>
@@ -6666,7 +6678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="89" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A89" s="1" t="inlineStr">
         <is>
           <t>Mimi Chen</t>
@@ -6742,7 +6754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="90" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A90" s="1" t="inlineStr">
         <is>
           <t>Will Ouyang</t>
@@ -6818,14 +6830,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="92" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A92" t="inlineStr">
         <is>
           <t>WEEK#</t>
         </is>
       </c>
     </row>
-    <row r="93" ht="39.75" customHeight="1" s="4" thickBot="1">
+    <row r="93" ht="39.75" customHeight="1" s="5" thickBot="1">
       <c r="A93" s="1" t="inlineStr">
         <is>
           <t>VS 'TEAM'</t>
@@ -6927,7 +6939,7 @@
         </is>
       </c>
     </row>
-    <row r="94" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="94" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A94" s="1" t="inlineStr">
         <is>
           <t>Brandon Chan</t>
@@ -7003,7 +7015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="95" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A95" s="1" t="inlineStr">
         <is>
           <t>Callum Ashton</t>
@@ -7079,7 +7091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="96" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A96" s="1" t="inlineStr">
         <is>
           <t>Daniel Park</t>
@@ -7155,7 +7167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="97" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A97" s="1" t="inlineStr">
         <is>
           <t>Deidre Truong</t>
@@ -7231,7 +7243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="98" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A98" s="1" t="inlineStr">
         <is>
           <t>Edward Kang</t>
@@ -7307,7 +7319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="99" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A99" s="1" t="inlineStr">
         <is>
           <t>Kevin Ma</t>
@@ -7383,7 +7395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="100" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A100" s="1" t="inlineStr">
         <is>
           <t>Kevin Tang</t>
@@ -7459,7 +7471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="101" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A101" s="1" t="inlineStr">
         <is>
           <t>Lachlan Denham</t>
@@ -7535,7 +7547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="102" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A102" s="1" t="inlineStr">
         <is>
           <t>Mimi Chen</t>
@@ -7611,7 +7623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="103" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A103" s="1" t="inlineStr">
         <is>
           <t>Will Ouyang</t>
@@ -7687,14 +7699,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="105" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A105" t="inlineStr">
         <is>
           <t>WEEK#</t>
         </is>
       </c>
     </row>
-    <row r="106" ht="39.75" customHeight="1" s="4" thickBot="1">
+    <row r="106" ht="39.75" customHeight="1" s="5" thickBot="1">
       <c r="A106" s="1" t="inlineStr">
         <is>
           <t>VS 'TEAM'</t>
@@ -7796,7 +7808,7 @@
         </is>
       </c>
     </row>
-    <row r="107" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="107" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A107" s="1" t="inlineStr">
         <is>
           <t>Brandon Chan</t>
@@ -7872,7 +7884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="108" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A108" s="1" t="inlineStr">
         <is>
           <t>Callum Ashton</t>
@@ -7948,7 +7960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="109" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A109" s="1" t="inlineStr">
         <is>
           <t>Daniel Park</t>
@@ -8024,7 +8036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="110" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A110" s="1" t="inlineStr">
         <is>
           <t>Deidre Truong</t>
@@ -8100,7 +8112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="111" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A111" s="1" t="inlineStr">
         <is>
           <t>Edward Kang</t>
@@ -8176,7 +8188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="112" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A112" s="1" t="inlineStr">
         <is>
           <t>Kevin Ma</t>
@@ -8252,7 +8264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="113" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A113" s="1" t="inlineStr">
         <is>
           <t>Kevin Tang</t>
@@ -8328,7 +8340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="114" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A114" s="1" t="inlineStr">
         <is>
           <t>Lachlan Denham</t>
@@ -8404,7 +8416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="115" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A115" s="1" t="inlineStr">
         <is>
           <t>Mimi Chen</t>
@@ -8480,7 +8492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="116" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A116" s="1" t="inlineStr">
         <is>
           <t>Will Ouyang</t>
@@ -8556,14 +8568,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="118" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A118" t="inlineStr">
         <is>
           <t>WEEK#</t>
         </is>
       </c>
     </row>
-    <row r="119" ht="39.75" customHeight="1" s="4" thickBot="1">
+    <row r="119" ht="39.75" customHeight="1" s="5" thickBot="1">
       <c r="A119" s="1" t="inlineStr">
         <is>
           <t>VS 'TEAM'</t>
@@ -8665,7 +8677,7 @@
         </is>
       </c>
     </row>
-    <row r="120" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="120" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A120" s="1" t="inlineStr">
         <is>
           <t>Brandon Chan</t>
@@ -8741,7 +8753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="121" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A121" s="1" t="inlineStr">
         <is>
           <t>Callum Ashton</t>
@@ -8817,7 +8829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="122" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A122" s="1" t="inlineStr">
         <is>
           <t>Daniel Park</t>
@@ -8893,7 +8905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="123" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A123" s="1" t="inlineStr">
         <is>
           <t>Deidre Truong</t>
@@ -8969,7 +8981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="124" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A124" s="1" t="inlineStr">
         <is>
           <t>Edward Kang</t>
@@ -9045,7 +9057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="125" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A125" s="1" t="inlineStr">
         <is>
           <t>Kevin Ma</t>
@@ -9121,7 +9133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="126" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A126" s="1" t="inlineStr">
         <is>
           <t>Kevin Tang</t>
@@ -9197,7 +9209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="127" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A127" s="1" t="inlineStr">
         <is>
           <t>Lachlan Denham</t>
@@ -9273,7 +9285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="128" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A128" s="1" t="inlineStr">
         <is>
           <t>Mimi Chen</t>
@@ -9349,7 +9361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="129" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A129" s="1" t="inlineStr">
         <is>
           <t>Will Ouyang</t>
@@ -9425,14 +9437,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="131" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A131" t="inlineStr">
         <is>
           <t>WEEK#</t>
         </is>
       </c>
     </row>
-    <row r="132" ht="39.75" customHeight="1" s="4" thickBot="1">
+    <row r="132" ht="39.75" customHeight="1" s="5" thickBot="1">
       <c r="A132" s="1" t="inlineStr">
         <is>
           <t>VS 'TEAM'</t>
@@ -9534,7 +9546,7 @@
         </is>
       </c>
     </row>
-    <row r="133" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="133" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A133" s="1" t="inlineStr">
         <is>
           <t>Brandon Chan</t>
@@ -9610,7 +9622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="134" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A134" s="1" t="inlineStr">
         <is>
           <t>Callum Ashton</t>
@@ -9686,7 +9698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="135" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A135" s="1" t="inlineStr">
         <is>
           <t>Daniel Park</t>
@@ -9762,7 +9774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="136" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A136" s="1" t="inlineStr">
         <is>
           <t>Deidre Truong</t>
@@ -9838,7 +9850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="137" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A137" s="1" t="inlineStr">
         <is>
           <t>Edward Kang</t>
@@ -9914,7 +9926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" ht="15.75" customHeight="1" s="4" thickBot="1">
+    <row r="138" ht="15.75" customHeight="1" s="5" thickBot="1">
       <c r="A138" s="1" t="inlineStr">
         <is>
           <t>Kevin Ma</t>
@@ -9990,7 +10002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="139" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A139" s="1" t="inlineStr">
         <is>
           <t>Kevin Tang</t>
@@ -10066,7 +10078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="140" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A140" s="1" t="inlineStr">
         <is>
           <t>Lachlan Denham</t>
@@ -10142,7 +10154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="141" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A141" s="1" t="inlineStr">
         <is>
           <t>Mimi Chen</t>
@@ -10218,7 +10230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" ht="27" customHeight="1" s="4" thickBot="1">
+    <row r="142" ht="27" customHeight="1" s="5" thickBot="1">
       <c r="A142" s="1" t="inlineStr">
         <is>
           <t>Will Ouyang</t>
@@ -10306,32 +10318,1214 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Week 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>VS 'TEAM'</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Serve Error</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Serve Success</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Serve %</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Receive Errors</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Receive Passes</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Receive %</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Set Errors</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Set Success</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Set %</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Spike Errors</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Spike Success</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Hit %</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Tip Errors</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Tip Success</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Tip %</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Block Errors</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Block Success</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Block %</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Faults</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Week 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>VS 'TEAM'</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Serve Error</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Serve Success</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Serve %</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Receive Errors</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Receive Passes</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Receive %</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Set Errors</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Set Success</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Set %</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Spike Errors</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Spike Success</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Hit %</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Tip Errors</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Tip Success</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Tip %</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Block Errors</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Block Success</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Block %</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Faults</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Week 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>VS 'TEAM'</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Serve Error</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Serve Success</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Serve %</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Receive Errors</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Receive Passes</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Receive %</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Set Errors</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Set Success</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Set %</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Spike Errors</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Spike Success</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Hit %</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Tip Errors</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Tip Success</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Tip %</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Block Errors</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Block Success</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>Block %</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>Faults</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Week 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>VS 'TEAM'</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Serve Error</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Serve Success</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Serve %</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Receive Errors</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Receive Passes</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Receive %</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Set Errors</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Set Success</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Set %</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Spike Errors</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Spike Success</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Hit %</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Tip Errors</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Tip Success</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Tip %</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Block Errors</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Block Success</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>Block %</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>Faults</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Week 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>VS 'TEAM'</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Serve Error</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Serve Success</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Serve %</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Receive Errors</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Receive Passes</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Receive %</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Set Errors</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Set Success</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Set %</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Spike Errors</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Spike Success</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Hit %</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Tip Errors</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>Tip Success</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Tip %</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Block Errors</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>Block Success</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>Block %</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>Faults</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Week 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>VS 'TEAM'</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Serve Error</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Serve Success</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Serve %</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Receive Errors</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Receive Passes</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Receive %</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Set Errors</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Set Success</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Set %</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Spike Errors</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Spike Success</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Hit %</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Tip Errors</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Tip Success</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Tip %</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Block Errors</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>Block Success</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>Block %</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>Faults</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Week 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>VS 'TEAM'</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Serve Error</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Serve Success</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Serve %</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Receive Errors</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Receive Passes</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Receive %</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Set Errors</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Set Success</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Set %</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Spike Errors</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Spike Success</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>Hit %</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Tip Errors</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>Tip Success</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>Tip %</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>Block Errors</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>Block Success</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>Block %</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>Faults</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Week 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>VS 'TEAM'</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Serve Error</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Serve Success</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Serve %</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Receive Errors</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Receive Passes</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Receive %</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Set Errors</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Set Success</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Set %</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Spike Errors</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Spike Success</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>Hit %</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>Tip Errors</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>Tip Success</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>Tip %</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>Block Errors</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>Block Success</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>Block %</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>Faults</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Week 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>VS 'TEAM'</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Serve Error</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Serve Success</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Serve %</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Receive Errors</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Receive Passes</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Receive %</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Set Errors</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Set Success</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Set %</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Spike Errors</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Spike Success</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>Hit %</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>Tip Errors</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>Tip Success</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>Tip %</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>Block Errors</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>Block Success</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>Block %</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>Faults</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Week 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>VS 'TEAM'</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Serve Error</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Serve Success</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Serve %</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Receive Errors</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Receive Passes</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Receive %</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Set Errors</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Set Success</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Set %</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Spike Errors</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Spike Success</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>Hit %</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>Tip Errors</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>Tip Success</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>Tip %</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>Block Errors</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>Block Success</t>
+        </is>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>Block %</t>
+        </is>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>Faults</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Week 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>VS 'TEAM'</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Serve Error</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Serve Success</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Serve %</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Receive Errors</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Receive Passes</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Receive %</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Set Errors</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Set Success</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Set %</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Spike Errors</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>Spike Success</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>Hit %</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>Tip Errors</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>Tip Success</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>Tip %</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>Block Errors</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>Block Success</t>
+        </is>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>Block %</t>
+        </is>
+      </c>
+      <c r="T32" t="inlineStr">
+        <is>
+          <t>Faults</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed extensive lag on player selection by editing usage of the buttonReset function
</commit_message>
<xml_diff>
--- a/data/volley_stats.xlsx
+++ b/data/volley_stats.xlsx
@@ -10880,8 +10880,10 @@
       <c r="C3" t="n">
         <v>0</v>
       </c>
-      <c r="D3" t="n">
-        <v>0</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -10889,8 +10891,10 @@
       <c r="F3" t="n">
         <v>0</v>
       </c>
-      <c r="G3" t="n">
-        <v>0</v>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -10898,8 +10902,10 @@
       <c r="I3" t="n">
         <v>0</v>
       </c>
-      <c r="J3" t="n">
-        <v>0</v>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="K3" t="n">
         <v>0</v>
@@ -10907,8 +10913,10 @@
       <c r="L3" t="n">
         <v>0</v>
       </c>
-      <c r="M3" t="n">
-        <v>0</v>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="N3" t="n">
         <v>0</v>
@@ -10916,8 +10924,10 @@
       <c r="O3" t="n">
         <v>0</v>
       </c>
-      <c r="P3" t="n">
-        <v>0</v>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="Q3" t="n">
         <v>0</v>
@@ -10925,8 +10935,10 @@
       <c r="R3" t="n">
         <v>0</v>
       </c>
-      <c r="S3" t="n">
-        <v>0</v>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="T3" t="n">
         <v>0</v>
@@ -10998,8 +11010,10 @@
       <c r="C4" t="n">
         <v>0</v>
       </c>
-      <c r="D4" t="n">
-        <v>0</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -11007,8 +11021,10 @@
       <c r="F4" t="n">
         <v>0</v>
       </c>
-      <c r="G4" t="n">
-        <v>0</v>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -11016,8 +11032,10 @@
       <c r="I4" t="n">
         <v>0</v>
       </c>
-      <c r="J4" t="n">
-        <v>0</v>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="K4" t="n">
         <v>0</v>
@@ -11025,8 +11043,10 @@
       <c r="L4" t="n">
         <v>0</v>
       </c>
-      <c r="M4" t="n">
-        <v>0</v>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="N4" t="n">
         <v>0</v>
@@ -11034,8 +11054,10 @@
       <c r="O4" t="n">
         <v>0</v>
       </c>
-      <c r="P4" t="n">
-        <v>0</v>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="Q4" t="n">
         <v>0</v>
@@ -11043,8 +11065,10 @@
       <c r="R4" t="n">
         <v>0</v>
       </c>
-      <c r="S4" t="n">
-        <v>0</v>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="T4" t="n">
         <v>0</v>
@@ -11116,8 +11140,10 @@
       <c r="C5" t="n">
         <v>0</v>
       </c>
-      <c r="D5" t="n">
-        <v>0</v>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -11125,8 +11151,10 @@
       <c r="F5" t="n">
         <v>0</v>
       </c>
-      <c r="G5" t="n">
-        <v>0</v>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -11134,8 +11162,10 @@
       <c r="I5" t="n">
         <v>0</v>
       </c>
-      <c r="J5" t="n">
-        <v>0</v>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="K5" t="n">
         <v>0</v>
@@ -11143,8 +11173,10 @@
       <c r="L5" t="n">
         <v>0</v>
       </c>
-      <c r="M5" t="n">
-        <v>0</v>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="N5" t="n">
         <v>0</v>
@@ -11152,8 +11184,10 @@
       <c r="O5" t="n">
         <v>0</v>
       </c>
-      <c r="P5" t="n">
-        <v>0</v>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="Q5" t="n">
         <v>0</v>
@@ -11161,8 +11195,10 @@
       <c r="R5" t="n">
         <v>0</v>
       </c>
-      <c r="S5" t="n">
-        <v>0</v>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="T5" t="n">
         <v>0</v>
@@ -11588,8 +11624,10 @@
       <c r="C9" t="n">
         <v>0</v>
       </c>
-      <c r="D9" t="n">
-        <v>0</v>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -11597,8 +11635,10 @@
       <c r="F9" t="n">
         <v>0</v>
       </c>
-      <c r="G9" t="n">
-        <v>0</v>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -11606,8 +11646,10 @@
       <c r="I9" t="n">
         <v>0</v>
       </c>
-      <c r="J9" t="n">
-        <v>0</v>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="K9" t="n">
         <v>0</v>
@@ -11615,8 +11657,10 @@
       <c r="L9" t="n">
         <v>0</v>
       </c>
-      <c r="M9" t="n">
-        <v>0</v>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="N9" t="n">
         <v>0</v>
@@ -11624,8 +11668,10 @@
       <c r="O9" t="n">
         <v>0</v>
       </c>
-      <c r="P9" t="n">
-        <v>0</v>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="Q9" t="n">
         <v>0</v>
@@ -11633,8 +11679,10 @@
       <c r="R9" t="n">
         <v>0</v>
       </c>
-      <c r="S9" t="n">
-        <v>0</v>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="T9" t="n">
         <v>0</v>
@@ -11706,8 +11754,10 @@
       <c r="C10" t="n">
         <v>0</v>
       </c>
-      <c r="D10" t="n">
-        <v>0</v>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -11715,8 +11765,10 @@
       <c r="F10" t="n">
         <v>0</v>
       </c>
-      <c r="G10" t="n">
-        <v>0</v>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -11724,8 +11776,10 @@
       <c r="I10" t="n">
         <v>0</v>
       </c>
-      <c r="J10" t="n">
-        <v>0</v>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="K10" t="n">
         <v>0</v>
@@ -11733,8 +11787,10 @@
       <c r="L10" t="n">
         <v>0</v>
       </c>
-      <c r="M10" t="n">
-        <v>0</v>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="N10" t="n">
         <v>0</v>
@@ -11742,8 +11798,10 @@
       <c r="O10" t="n">
         <v>0</v>
       </c>
-      <c r="P10" t="n">
-        <v>0</v>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="Q10" t="n">
         <v>0</v>
@@ -11751,8 +11809,10 @@
       <c r="R10" t="n">
         <v>0</v>
       </c>
-      <c r="S10" t="n">
-        <v>0</v>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="T10" t="n">
         <v>0</v>
@@ -11824,8 +11884,10 @@
       <c r="C11" t="n">
         <v>0</v>
       </c>
-      <c r="D11" t="n">
-        <v>0</v>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -11833,8 +11895,10 @@
       <c r="F11" t="n">
         <v>0</v>
       </c>
-      <c r="G11" t="n">
-        <v>0</v>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -11842,8 +11906,10 @@
       <c r="I11" t="n">
         <v>0</v>
       </c>
-      <c r="J11" t="n">
-        <v>0</v>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="K11" t="n">
         <v>0</v>
@@ -11851,8 +11917,10 @@
       <c r="L11" t="n">
         <v>0</v>
       </c>
-      <c r="M11" t="n">
-        <v>0</v>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="N11" t="n">
         <v>0</v>
@@ -11860,8 +11928,10 @@
       <c r="O11" t="n">
         <v>0</v>
       </c>
-      <c r="P11" t="n">
-        <v>0</v>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="Q11" t="n">
         <v>0</v>
@@ -11869,8 +11939,10 @@
       <c r="R11" t="n">
         <v>0</v>
       </c>
-      <c r="S11" t="n">
-        <v>0</v>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="T11" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Updated the statistics labels to match new format. Labels still need to be connected to excel sheet to display current values.
</commit_message>
<xml_diff>
--- a/data/volley_stats.xlsx
+++ b/data/volley_stats.xlsx
@@ -12449,8 +12449,10 @@
       <c r="C17" t="n">
         <v>0</v>
       </c>
-      <c r="D17" t="n">
-        <v>0</v>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -12458,8 +12460,10 @@
       <c r="F17" t="n">
         <v>0</v>
       </c>
-      <c r="G17" t="n">
-        <v>0</v>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -12467,8 +12471,10 @@
       <c r="I17" t="n">
         <v>0</v>
       </c>
-      <c r="J17" t="n">
-        <v>0</v>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="K17" t="n">
         <v>0</v>
@@ -12476,8 +12482,10 @@
       <c r="L17" t="n">
         <v>0</v>
       </c>
-      <c r="M17" t="n">
-        <v>0</v>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="N17" t="n">
         <v>0</v>
@@ -12485,8 +12493,10 @@
       <c r="O17" t="n">
         <v>0</v>
       </c>
-      <c r="P17" t="n">
-        <v>0</v>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="Q17" t="n">
         <v>0</v>
@@ -12494,8 +12504,10 @@
       <c r="R17" t="n">
         <v>0</v>
       </c>
-      <c r="S17" t="n">
-        <v>0</v>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="T17" t="n">
         <v>0</v>
@@ -15080,8 +15092,10 @@
       <c r="C41" t="n">
         <v>0</v>
       </c>
-      <c r="D41" t="n">
-        <v>0</v>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="E41" t="n">
         <v>0</v>
@@ -15089,8 +15103,10 @@
       <c r="F41" t="n">
         <v>0</v>
       </c>
-      <c r="G41" t="n">
-        <v>0</v>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="H41" t="n">
         <v>0</v>
@@ -15098,8 +15114,10 @@
       <c r="I41" t="n">
         <v>0</v>
       </c>
-      <c r="J41" t="n">
-        <v>0</v>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="K41" t="n">
         <v>0</v>
@@ -15107,8 +15125,10 @@
       <c r="L41" t="n">
         <v>0</v>
       </c>
-      <c r="M41" t="n">
-        <v>0</v>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="N41" t="n">
         <v>0</v>
@@ -15116,8 +15136,10 @@
       <c r="O41" t="n">
         <v>0</v>
       </c>
-      <c r="P41" t="n">
-        <v>0</v>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="Q41" t="n">
         <v>0</v>
@@ -15125,8 +15147,10 @@
       <c r="R41" t="n">
         <v>0</v>
       </c>
-      <c r="S41" t="n">
-        <v>0</v>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="T41" t="n">
         <v>0</v>
@@ -16105,8 +16129,10 @@
       <c r="C51" t="n">
         <v>0</v>
       </c>
-      <c r="D51" t="n">
-        <v>0</v>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="E51" t="n">
         <v>0</v>
@@ -16114,8 +16140,10 @@
       <c r="F51" t="n">
         <v>0</v>
       </c>
-      <c r="G51" t="n">
-        <v>0</v>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -16123,8 +16151,10 @@
       <c r="I51" t="n">
         <v>0</v>
       </c>
-      <c r="J51" t="n">
-        <v>0</v>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="K51" t="n">
         <v>0</v>
@@ -16132,8 +16162,10 @@
       <c r="L51" t="n">
         <v>0</v>
       </c>
-      <c r="M51" t="n">
-        <v>0</v>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="N51" t="n">
         <v>0</v>
@@ -16141,8 +16173,10 @@
       <c r="O51" t="n">
         <v>0</v>
       </c>
-      <c r="P51" t="n">
-        <v>0</v>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="Q51" t="n">
         <v>0</v>
@@ -16150,8 +16184,10 @@
       <c r="R51" t="n">
         <v>0</v>
       </c>
-      <c r="S51" t="n">
-        <v>0</v>
+      <c r="S51" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="T51" t="n">
         <v>0</v>
@@ -16223,8 +16259,10 @@
       <c r="C52" t="n">
         <v>0</v>
       </c>
-      <c r="D52" t="n">
-        <v>0</v>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="E52" t="n">
         <v>0</v>
@@ -16232,8 +16270,10 @@
       <c r="F52" t="n">
         <v>0</v>
       </c>
-      <c r="G52" t="n">
-        <v>0</v>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="H52" t="n">
         <v>0</v>
@@ -16241,8 +16281,10 @@
       <c r="I52" t="n">
         <v>0</v>
       </c>
-      <c r="J52" t="n">
-        <v>0</v>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="K52" t="n">
         <v>0</v>
@@ -16250,8 +16292,10 @@
       <c r="L52" t="n">
         <v>0</v>
       </c>
-      <c r="M52" t="n">
-        <v>0</v>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="N52" t="n">
         <v>0</v>
@@ -16259,8 +16303,10 @@
       <c r="O52" t="n">
         <v>0</v>
       </c>
-      <c r="P52" t="n">
-        <v>0</v>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="Q52" t="n">
         <v>0</v>
@@ -16268,8 +16314,10 @@
       <c r="R52" t="n">
         <v>0</v>
       </c>
-      <c r="S52" t="n">
-        <v>0</v>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="T52" t="n">
         <v>0</v>
@@ -16341,8 +16389,10 @@
       <c r="C53" t="n">
         <v>0</v>
       </c>
-      <c r="D53" t="n">
-        <v>0</v>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="E53" t="n">
         <v>0</v>
@@ -16350,8 +16400,10 @@
       <c r="F53" t="n">
         <v>0</v>
       </c>
-      <c r="G53" t="n">
-        <v>0</v>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -16359,8 +16411,10 @@
       <c r="I53" t="n">
         <v>0</v>
       </c>
-      <c r="J53" t="n">
-        <v>0</v>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="K53" t="n">
         <v>0</v>
@@ -16368,8 +16422,10 @@
       <c r="L53" t="n">
         <v>0</v>
       </c>
-      <c r="M53" t="n">
-        <v>0</v>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="N53" t="n">
         <v>0</v>
@@ -16377,8 +16433,10 @@
       <c r="O53" t="n">
         <v>0</v>
       </c>
-      <c r="P53" t="n">
-        <v>0</v>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="Q53" t="n">
         <v>0</v>
@@ -16386,8 +16444,10 @@
       <c r="R53" t="n">
         <v>0</v>
       </c>
-      <c r="S53" t="n">
-        <v>0</v>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="T53" t="n">
         <v>0</v>
@@ -16459,8 +16519,10 @@
       <c r="C54" t="n">
         <v>0</v>
       </c>
-      <c r="D54" t="n">
-        <v>0</v>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="E54" t="n">
         <v>0</v>
@@ -16468,8 +16530,10 @@
       <c r="F54" t="n">
         <v>0</v>
       </c>
-      <c r="G54" t="n">
-        <v>0</v>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="H54" t="n">
         <v>0</v>
@@ -16477,8 +16541,10 @@
       <c r="I54" t="n">
         <v>0</v>
       </c>
-      <c r="J54" t="n">
-        <v>0</v>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="K54" t="n">
         <v>0</v>
@@ -16486,8 +16552,10 @@
       <c r="L54" t="n">
         <v>0</v>
       </c>
-      <c r="M54" t="n">
-        <v>0</v>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="N54" t="n">
         <v>0</v>
@@ -16495,8 +16563,10 @@
       <c r="O54" t="n">
         <v>0</v>
       </c>
-      <c r="P54" t="n">
-        <v>0</v>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="Q54" t="n">
         <v>0</v>
@@ -16504,8 +16574,10 @@
       <c r="R54" t="n">
         <v>0</v>
       </c>
-      <c r="S54" t="n">
-        <v>0</v>
+      <c r="S54" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="T54" t="n">
         <v>0</v>
@@ -16577,8 +16649,10 @@
       <c r="C55" t="n">
         <v>0</v>
       </c>
-      <c r="D55" t="n">
-        <v>0</v>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="E55" t="n">
         <v>0</v>
@@ -16586,8 +16660,10 @@
       <c r="F55" t="n">
         <v>0</v>
       </c>
-      <c r="G55" t="n">
-        <v>0</v>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -16595,8 +16671,10 @@
       <c r="I55" t="n">
         <v>0</v>
       </c>
-      <c r="J55" t="n">
-        <v>0</v>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="K55" t="n">
         <v>0</v>
@@ -16604,8 +16682,10 @@
       <c r="L55" t="n">
         <v>0</v>
       </c>
-      <c r="M55" t="n">
-        <v>0</v>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="N55" t="n">
         <v>0</v>
@@ -16613,8 +16693,10 @@
       <c r="O55" t="n">
         <v>0</v>
       </c>
-      <c r="P55" t="n">
-        <v>0</v>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="Q55" t="n">
         <v>0</v>
@@ -16622,8 +16704,10 @@
       <c r="R55" t="n">
         <v>0</v>
       </c>
-      <c r="S55" t="n">
-        <v>0</v>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="T55" t="n">
         <v>0</v>
@@ -16695,8 +16779,10 @@
       <c r="C56" t="n">
         <v>0</v>
       </c>
-      <c r="D56" t="n">
-        <v>0</v>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="E56" t="n">
         <v>0</v>
@@ -16704,8 +16790,10 @@
       <c r="F56" t="n">
         <v>0</v>
       </c>
-      <c r="G56" t="n">
-        <v>0</v>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="H56" t="n">
         <v>0</v>
@@ -16713,8 +16801,10 @@
       <c r="I56" t="n">
         <v>0</v>
       </c>
-      <c r="J56" t="n">
-        <v>0</v>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="K56" t="n">
         <v>0</v>
@@ -16722,8 +16812,10 @@
       <c r="L56" t="n">
         <v>0</v>
       </c>
-      <c r="M56" t="n">
-        <v>0</v>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="N56" t="n">
         <v>0</v>
@@ -16731,8 +16823,10 @@
       <c r="O56" t="n">
         <v>0</v>
       </c>
-      <c r="P56" t="n">
-        <v>0</v>
+      <c r="P56" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="Q56" t="n">
         <v>0</v>
@@ -16740,8 +16834,10 @@
       <c r="R56" t="n">
         <v>0</v>
       </c>
-      <c r="S56" t="n">
-        <v>0</v>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="T56" t="n">
         <v>0</v>
@@ -16813,8 +16909,10 @@
       <c r="C57" t="n">
         <v>0</v>
       </c>
-      <c r="D57" t="n">
-        <v>0</v>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="E57" t="n">
         <v>0</v>
@@ -16822,8 +16920,10 @@
       <c r="F57" t="n">
         <v>0</v>
       </c>
-      <c r="G57" t="n">
-        <v>0</v>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="H57" t="n">
         <v>0</v>
@@ -16831,8 +16931,10 @@
       <c r="I57" t="n">
         <v>0</v>
       </c>
-      <c r="J57" t="n">
-        <v>0</v>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="K57" t="n">
         <v>0</v>
@@ -16840,8 +16942,10 @@
       <c r="L57" t="n">
         <v>0</v>
       </c>
-      <c r="M57" t="n">
-        <v>0</v>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="N57" t="n">
         <v>0</v>
@@ -16849,8 +16953,10 @@
       <c r="O57" t="n">
         <v>0</v>
       </c>
-      <c r="P57" t="n">
-        <v>0</v>
+      <c r="P57" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="Q57" t="n">
         <v>0</v>
@@ -16858,8 +16964,10 @@
       <c r="R57" t="n">
         <v>0</v>
       </c>
-      <c r="S57" t="n">
-        <v>0</v>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="T57" t="n">
         <v>0</v>
@@ -16931,8 +17039,10 @@
       <c r="C58" t="n">
         <v>0</v>
       </c>
-      <c r="D58" t="n">
-        <v>0</v>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="E58" t="n">
         <v>0</v>
@@ -16940,8 +17050,10 @@
       <c r="F58" t="n">
         <v>0</v>
       </c>
-      <c r="G58" t="n">
-        <v>0</v>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -16949,8 +17061,10 @@
       <c r="I58" t="n">
         <v>0</v>
       </c>
-      <c r="J58" t="n">
-        <v>0</v>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="K58" t="n">
         <v>0</v>
@@ -16958,8 +17072,10 @@
       <c r="L58" t="n">
         <v>0</v>
       </c>
-      <c r="M58" t="n">
-        <v>0</v>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="N58" t="n">
         <v>0</v>
@@ -16967,8 +17083,10 @@
       <c r="O58" t="n">
         <v>0</v>
       </c>
-      <c r="P58" t="n">
-        <v>0</v>
+      <c r="P58" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="Q58" t="n">
         <v>0</v>
@@ -16976,8 +17094,10 @@
       <c r="R58" t="n">
         <v>0</v>
       </c>
-      <c r="S58" t="n">
-        <v>0</v>
+      <c r="S58" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="T58" t="n">
         <v>0</v>
@@ -17049,8 +17169,10 @@
       <c r="C59" t="n">
         <v>0</v>
       </c>
-      <c r="D59" t="n">
-        <v>0</v>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="E59" t="n">
         <v>0</v>
@@ -17058,8 +17180,10 @@
       <c r="F59" t="n">
         <v>0</v>
       </c>
-      <c r="G59" t="n">
-        <v>0</v>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -17067,8 +17191,10 @@
       <c r="I59" t="n">
         <v>0</v>
       </c>
-      <c r="J59" t="n">
-        <v>0</v>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="K59" t="n">
         <v>0</v>
@@ -17076,8 +17202,10 @@
       <c r="L59" t="n">
         <v>0</v>
       </c>
-      <c r="M59" t="n">
-        <v>0</v>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="N59" t="n">
         <v>0</v>
@@ -17085,8 +17213,10 @@
       <c r="O59" t="n">
         <v>0</v>
       </c>
-      <c r="P59" t="n">
-        <v>0</v>
+      <c r="P59" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="Q59" t="n">
         <v>0</v>
@@ -17094,8 +17224,10 @@
       <c r="R59" t="n">
         <v>0</v>
       </c>
-      <c r="S59" t="n">
-        <v>0</v>
+      <c r="S59" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="T59" t="n">
         <v>0</v>

</xml_diff>